<commit_message>
Updated Power Pins and Header Layout
</commit_message>
<xml_diff>
--- a/Board/#Resources/#Resources.xlsx
+++ b/Board/#Resources/#Resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\#Code\Basketball_Shot_Trainer\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\#Code\Basketball_Shot_Trainer\Board\#Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52320CCE-FAE2-4361-8DAB-54D0739FE4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CD8D5B-04AA-4161-B1C1-4813E6C9A71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>BLE Board</t>
   </si>
@@ -63,16 +63,102 @@
   </si>
   <si>
     <t>https://learn.adafruit.com/adafruit-bno055-absolute-orientation-sensor/pinouts</t>
+  </si>
+  <si>
+    <t>6 pin female</t>
+  </si>
+  <si>
+    <t>8 pin female</t>
+  </si>
+  <si>
+    <t>12 pin female</t>
+  </si>
+  <si>
+    <t>6 pin male</t>
+  </si>
+  <si>
+    <t>8 pin male</t>
+  </si>
+  <si>
+    <t>12 pin male</t>
+  </si>
+  <si>
+    <t>10k resistor 0603</t>
+  </si>
+  <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t>RGB Resistor</t>
+  </si>
+  <si>
+    <t>PWR LED</t>
+  </si>
+  <si>
+    <t>PWR Resistor</t>
+  </si>
+  <si>
+    <t>Coin Cell Holder</t>
+  </si>
+  <si>
+    <t>Coin Cell</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>4.7uF Cap_16V</t>
+  </si>
+  <si>
+    <t>1uF Cap 0603</t>
+  </si>
+  <si>
+    <t>0.1uF Cap 0603</t>
+  </si>
+  <si>
+    <t>5v Regulator</t>
+  </si>
+  <si>
+    <t>6 Pin IMU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/91601-412ALF/2713716</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/91601-308LF/1535152</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/91614-306ALF/1536169</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/77311-401-06LF/1657857</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/68002-208HLF/1878507</t>
+  </si>
+  <si>
+    <t>(2 6 pins)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +181,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,14 +547,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DB5329-B5EB-4B52-AE8E-BED08A60CDF8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{65DAFF53-7DA5-4933-A569-BA8DEACA1483}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{6DC26843-32AD-4344-BEC4-D8322A951F4A}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{BE700257-2203-4DE1-ADCD-564D9873959C}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{282A3497-5042-4D6E-A9BE-0482290BDB2D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add \CAD\Old STP Files
</commit_message>
<xml_diff>
--- a/Board/#Resources/#Resources.xlsx
+++ b/Board/#Resources/#Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\#Code\Basketball_Shot_Trainer\Board\#Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CD8D5B-04AA-4161-B1C1-4813E6C9A71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE2473E-CAC4-4569-AC28-B6DD7209A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>BLE Board</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>(2 6 pins)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/american-opto-plus-led/L171L-GC/12325425</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13:N14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +628,9 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Updated RevA Parts List/Digikey Order 1
</commit_message>
<xml_diff>
--- a/Board/#Resources/#Resources.xlsx
+++ b/Board/#Resources/#Resources.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\#Code\Basketball_Shot_Trainer\Board\#Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AAA3B4-3FEB-4D80-8E15-EB262ADBA780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44946BD-5FED-4C06-9696-5B5D1CDB793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="1" r:id="rId1"/>
     <sheet name="RevA Details" sheetId="2" r:id="rId2"/>
     <sheet name="Relevant Parts" sheetId="3" r:id="rId3"/>
+    <sheet name="Order 1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
   <si>
     <t>BLE Board</t>
   </si>
@@ -107,9 +108,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>Regulator</t>
-  </si>
-  <si>
     <t>4.7uF Cap_16V</t>
   </si>
   <si>
@@ -122,9 +120,6 @@
     <t>5v Regulator</t>
   </si>
   <si>
-    <t>6 Pin IMU</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/91601-412ALF/2713716</t>
   </si>
   <si>
@@ -146,17 +141,224 @@
     <t>https://www.digikey.com/en/products/detail/american-opto-plus-led/L171L-GC/12325425</t>
   </si>
   <si>
-    <t>digikey 1027</t>
-  </si>
-  <si>
     <t>cr2330</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-610/11655708</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/harvatek-corporation/B3803FCH-20C001112U1930/13588742</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM185R61E105KA12D/5026383</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/walsin-technology-corporation/0603B104K101CT/1292-1392-1-ND/9355396</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM1117IMPX-5-0-NOPB/3440161</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/avx-corporation/TAJA475M016RNJ/808808</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nidec-copal-electronics/CFS-0102TA/12142641</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/1027/49724</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-bsg/CR2330/107117</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sunled/XZCDGK53W-8VF/10449775</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/susumu/RR0816P-152-D/432189</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-PB3D2000V/6212984</t>
+  </si>
+  <si>
+    <t>6-cable</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/30-00510/6245003</t>
+  </si>
+  <si>
+    <t>28-wire-red</t>
+  </si>
+  <si>
+    <t>28-wire-black</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/30-01783/13998447</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/30-01782/13998326</t>
+  </si>
+  <si>
+    <t>6 Pin IMU board</t>
+  </si>
+  <si>
+    <t>6 pin IMU cable</t>
+  </si>
+  <si>
+    <t>6 pin IMU Crimps?</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>6 Pin Female Header</t>
+  </si>
+  <si>
+    <t>609-4475-1-ND</t>
+  </si>
+  <si>
+    <t>8 Pin Female Header</t>
+  </si>
+  <si>
+    <t>609-4966-ND</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>12 Pin Female Header</t>
+  </si>
+  <si>
+    <t>609-4414-1-ND</t>
+  </si>
+  <si>
+    <t>6 Pin Male Header</t>
+  </si>
+  <si>
+    <t>8 Pin Male Header</t>
+  </si>
+  <si>
+    <t>10K Resistor</t>
+  </si>
+  <si>
+    <t>Incorrect!!!</t>
+  </si>
+  <si>
+    <t>3147-B3803FCH-20C001112U1930CT-ND</t>
+  </si>
+  <si>
+    <t>2368-SR1-0603-610-ND</t>
+  </si>
+  <si>
+    <t>200 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>P20201CT-ND</t>
+  </si>
+  <si>
+    <t>Power LED</t>
+  </si>
+  <si>
+    <t>1497-XZCDGK53W-8VFCT-ND</t>
+  </si>
+  <si>
+    <t>1.5K Resistor</t>
+  </si>
+  <si>
+    <t>RR08P1.5KDCT-ND</t>
+  </si>
+  <si>
+    <t>23mm Coin Cell Holder</t>
+  </si>
+  <si>
+    <t>36-1027-ND</t>
+  </si>
+  <si>
+    <t>CR2330 Batteries</t>
+  </si>
+  <si>
+    <t>P111-ND</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>563-CFS-0102TACT-ND</t>
+  </si>
+  <si>
+    <t>4.7uF Tantalum Capacitor</t>
+  </si>
+  <si>
+    <t>478-3032-1-ND</t>
+  </si>
+  <si>
+    <t>1uF Capacitor</t>
+  </si>
+  <si>
+    <t>490-10021-1-ND</t>
+  </si>
+  <si>
+    <t>0.1uF Capacitor</t>
+  </si>
+  <si>
+    <t>1292-1392-1-ND</t>
+  </si>
+  <si>
+    <t>5V Regulator</t>
+  </si>
+  <si>
+    <t>LM1117IMPX-5.0/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>28/6 Wire 1m</t>
+  </si>
+  <si>
+    <t>T1347-1-ND</t>
+  </si>
+  <si>
+    <t>6 Pin IMU Board Conn.</t>
+  </si>
+  <si>
+    <t>6 Pin IMU Cable Conn.</t>
+  </si>
+  <si>
+    <t>6 Pin IMU Crimps</t>
+  </si>
+  <si>
+    <t>28 AWG Hookup Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Digikey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +374,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +391,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,14 +399,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -556,142 +785,207 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DB5329-B5EB-4B52-AE8E-BED08A60CDF8}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -700,7 +994,502 @@
     <hyperlink ref="B4" r:id="rId2" xr:uid="{6DC26843-32AD-4344-BEC4-D8322A951F4A}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{BE700257-2203-4DE1-ADCD-564D9873959C}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{282A3497-5042-4D6E-A9BE-0482290BDB2D}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{3B482E8F-3EB5-480A-835A-01E7263CDDB9}"/>
+    <hyperlink ref="D13" r:id="rId6" xr:uid="{948E4952-6DA7-4E2C-B924-E987B44DF58B}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{835D7C14-4215-46CF-A7B4-FCA7786CA17D}"/>
+    <hyperlink ref="B1" r:id="rId8" xr:uid="{FC9BB88D-4609-4504-B301-F722AD39FEE4}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{CFA0B0BB-6EF7-4AF9-AB78-E87A37946418}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{D29CD3A2-0676-4D10-9067-3978CEF544DA}"/>
+    <hyperlink ref="C10" r:id="rId11" xr:uid="{2C616405-ED8C-49A9-9C40-CD32C9B46A74}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{95BC884C-A718-4854-B0FC-C9AD2785811F}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{7F2CAEE5-F5F1-43CE-86AB-F672AB4C9DCD}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{9AE5BC9A-0E5D-4341-B3EB-54A51DE1CFCD}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{C1BFD008-EDE4-49C8-B7E3-290062FC5DA2}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{42026E6E-0378-465B-B429-3A68D888CEA2}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{A1934A82-A533-4C24-A3EB-90DA3BB31C33}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{8D21C30F-EC4C-4C1D-9748-4E9EBC06AA45}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{B3FB6EEA-696F-4AB8-85D6-31AF98375A95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B02D89F-213F-41FC-B164-02F6E549A093}">
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="5">
+        <f>SUM(E:E)</f>
+        <v>42.57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.42</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4*C4</f>
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E25" si="0">D5*C5</f>
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.65</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>5.76</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>1.35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.246</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>2.46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="3">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>2.82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.58</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>7.74</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Old .SLDPRT Files
</commit_message>
<xml_diff>
--- a/Board/#Resources/#Resources.xlsx
+++ b/Board/#Resources/#Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\#Code\Basketball_Shot_Trainer\Board\#Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44946BD-5FED-4C06-9696-5B5D1CDB793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231B1EB-3ED4-43A2-A621-5DCEF880DCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
   <si>
     <t>BLE Board</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t xml:space="preserve">  Digikey</t>
+  </si>
+  <si>
+    <t>Shipping Estimate</t>
+  </si>
+  <si>
+    <t>N/a                                                                        ~</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B02D89F-213F-41FC-B164-02F6E549A093}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:E25" si="0">D5*C5</f>
+        <f t="shared" ref="E5:E26" si="0">D5*C5</f>
         <v>2.58</v>
       </c>
     </row>
@@ -1484,6 +1490,21 @@
         <v>1</v>
       </c>
       <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixed Resources.xlsx, Correct 6 Pin Header
</commit_message>
<xml_diff>
--- a/Board/#Resources/#Resources.xlsx
+++ b/Board/#Resources/#Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\#Code\Basketball_Shot_Trainer\Board\#Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DEF24B-1221-4A63-85F7-DA8BB26DE96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6818E-0B2C-4DB1-BF92-01B2DC9494E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="110">
   <si>
     <t>BLE Board</t>
   </si>
@@ -268,9 +268,6 @@
     <t>6 Pin Female Header</t>
   </si>
   <si>
-    <t>609-4475-1-ND</t>
-  </si>
-  <si>
     <t>8 Pin Female Header</t>
   </si>
   <si>
@@ -392,6 +389,12 @@
   </si>
   <si>
     <t>YAG2321CT-ND</t>
+  </si>
+  <si>
+    <t>609-6018-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/91601-306LF/1535606</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1018,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1081,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,20 +1096,20 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(E:E)</f>
-        <v>48.31</v>
+        <v>46.67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,28 +1147,28 @@
         <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="C4" s="3">
-        <v>1.42</v>
+        <v>1.01</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4" s="3">
         <f>D4*C4</f>
-        <v>5.68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
+        <v>4.04</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
       </c>
       <c r="C5" s="3">
         <v>1.29</v>
@@ -1177,16 +1180,16 @@
         <f t="shared" ref="E5:E21" si="0">D5*C5</f>
         <v>2.58</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
       </c>
       <c r="C6" s="3">
         <v>2.65</v>
@@ -1198,16 +1201,16 @@
         <f t="shared" si="0"/>
         <v>5.3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="3">
         <v>0.48399999999999999</v>
@@ -1220,15 +1223,15 @@
         <v>4.84</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="3">
         <v>0.24</v>
@@ -1241,15 +1244,15 @@
         <v>0.48</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="3">
         <v>5.8999999999999997E-2</v>
@@ -1262,7 +1265,7 @@
         <v>1.18</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1270,7 +1273,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3">
         <v>0.21</v>
@@ -1288,10 +1291,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
       </c>
       <c r="C11" s="3">
         <v>0.13500000000000001</v>
@@ -1309,10 +1312,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
         <v>79</v>
-      </c>
-      <c r="B12" t="s">
-        <v>80</v>
       </c>
       <c r="C12" s="3">
         <v>0.63</v>
@@ -1330,10 +1333,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
         <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>82</v>
       </c>
       <c r="C13" s="3">
         <v>8.8999999999999996E-2</v>
@@ -1351,10 +1354,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
       </c>
       <c r="C14" s="3">
         <v>1.55</v>
@@ -1372,10 +1375,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
         <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>86</v>
       </c>
       <c r="C15" s="3">
         <v>1.44</v>
@@ -1393,10 +1396,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
         <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
       </c>
       <c r="C16" s="3">
         <v>0.79</v>
@@ -1414,10 +1417,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="3">
         <v>0.56000000000000005</v>
@@ -1430,15 +1433,15 @@
         <v>1.6800000000000002</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
         <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
       </c>
       <c r="C18" s="3">
         <v>0.246</v>
@@ -1456,10 +1459,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
         <v>92</v>
-      </c>
-      <c r="B19" t="s">
-        <v>93</v>
       </c>
       <c r="C19" s="3">
         <v>9.1999999999999998E-2</v>
@@ -1477,10 +1480,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
         <v>94</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
       </c>
       <c r="C20" s="3">
         <v>1.41</v>
@@ -1498,10 +1501,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
       </c>
       <c r="C21" s="3">
         <v>6.99</v>
@@ -1519,9 +1522,12 @@
     <hyperlink ref="G7" r:id="rId1" xr:uid="{DD62920D-A18B-4952-96AF-F0FE1D9B58BB}"/>
     <hyperlink ref="G17" r:id="rId2" xr:uid="{94213418-B07C-449C-9B07-F47AD55A361B}"/>
     <hyperlink ref="G9" r:id="rId3" xr:uid="{072CCE3A-AE80-4A7E-AD80-EE71E08BAA4C}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{D96FDD44-CDFF-4F97-BA0B-3B37E331C584}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{B4AD035A-77EA-4550-B3AB-97EF1B7F376E}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{CF64B061-5C3F-4ACB-B656-7F300ED58188}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>